<commit_message>
Created new table with aggregated emails for llm finetuning
</commit_message>
<xml_diff>
--- a/data/etl/Extracted_Employee_Emails_and_Roles.xlsx
+++ b/data/etl/Extracted_Employee_Emails_and_Roles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au664431_uni_au_dk/Documents/Speciale/Speciale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{339EBD5D-1E87-4FB4-8753-4B6FE61DD527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2D69B34-56BE-9D4E-B1D4-EB24F0C06452}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{339EBD5D-1E87-4FB4-8753-4B6FE61DD527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF6FECAC-9ADC-C14E-8D9E-25912658D632}"/>
   <bookViews>
-    <workbookView xWindow="-39500" yWindow="2980" windowWidth="34280" windowHeight="24920" xr2:uid="{12E394CB-B8C8-4C17-8D20-FB3F763C7507}"/>
+    <workbookView xWindow="-51200" yWindow="3280" windowWidth="51200" windowHeight="27220" xr2:uid="{12E394CB-B8C8-4C17-8D20-FB3F763C7507}"/>
   </bookViews>
   <sheets>
     <sheet name="Extracted_Employee_Emails_and_R" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="275">
   <si>
     <t>Name</t>
   </si>
@@ -787,9 +787,6 @@
     <t>it</t>
   </si>
   <si>
-    <t>transport</t>
-  </si>
-  <si>
     <t>cutting@dacapo,com</t>
   </si>
   <si>
@@ -824,6 +821,30 @@
   </si>
   <si>
     <t>transport@dacapo.com</t>
+  </si>
+  <si>
+    <t>consnl@dacapo.com</t>
+  </si>
+  <si>
+    <t>goodsreception@dacapo.com</t>
+  </si>
+  <si>
+    <t>dkwm@dacapo.com</t>
+  </si>
+  <si>
+    <t>ive@dacapo.com</t>
+  </si>
+  <si>
+    <t>cutting@dacapo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warehouse </t>
+  </si>
+  <si>
+    <t>additional information</t>
+  </si>
+  <si>
+    <t>production</t>
   </si>
 </sst>
 </file>
@@ -1382,6 +1403,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1699,18 +1724,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB866C6-E2C8-4DCC-9174-1219AC93492B}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1721,10 +1747,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1738,7 +1764,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -1753,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -1768,7 +1794,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -1783,7 +1809,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -1798,7 +1824,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1813,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1828,7 +1854,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -1843,7 +1869,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -1858,7 +1884,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -1873,7 +1899,7 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -1888,7 +1914,7 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -1903,7 +1929,7 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1918,7 +1944,7 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1933,7 +1959,7 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1948,7 +1974,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -1963,7 +1989,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -1978,7 +2004,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -1993,7 +2019,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -2008,7 +2034,7 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -2023,7 +2049,7 @@
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -2038,7 +2064,7 @@
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -2053,7 +2079,7 @@
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -2068,7 +2094,7 @@
         <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -2083,7 +2109,7 @@
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -2098,7 +2124,7 @@
         <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E26" s="3"/>
     </row>
@@ -2113,7 +2139,7 @@
         <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E27" s="3"/>
     </row>
@@ -2128,7 +2154,7 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E28" s="3"/>
     </row>
@@ -2143,7 +2169,7 @@
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E29" s="3"/>
     </row>
@@ -2158,7 +2184,7 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E30" s="3"/>
     </row>
@@ -2173,7 +2199,7 @@
         <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -2188,7 +2214,7 @@
         <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -2203,7 +2229,7 @@
         <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E33" s="3"/>
     </row>
@@ -2218,7 +2244,7 @@
         <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E34" s="3"/>
     </row>
@@ -2233,7 +2259,7 @@
         <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E35" s="3"/>
     </row>
@@ -2248,7 +2274,7 @@
         <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E36" s="3"/>
     </row>
@@ -2263,7 +2289,7 @@
         <v>68</v>
       </c>
       <c r="D37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E37" s="3"/>
     </row>
@@ -2278,7 +2304,7 @@
         <v>70</v>
       </c>
       <c r="D38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E38" s="3"/>
     </row>
@@ -2293,7 +2319,7 @@
         <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E39" s="3"/>
     </row>
@@ -2308,7 +2334,7 @@
         <v>243</v>
       </c>
       <c r="D40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E40" s="3"/>
     </row>
@@ -2323,7 +2349,7 @@
         <v>242</v>
       </c>
       <c r="D41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E41" s="3"/>
     </row>
@@ -2338,7 +2364,7 @@
         <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E42" s="3"/>
     </row>
@@ -2353,7 +2379,7 @@
         <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E43" s="3"/>
     </row>
@@ -2368,7 +2394,7 @@
         <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E44" s="3"/>
     </row>
@@ -2383,7 +2409,7 @@
         <v>85</v>
       </c>
       <c r="D45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E45" s="3"/>
     </row>
@@ -2398,7 +2424,7 @@
         <v>87</v>
       </c>
       <c r="D46" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E46" s="3"/>
     </row>
@@ -2413,7 +2439,7 @@
         <v>88</v>
       </c>
       <c r="D47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E47" s="3"/>
     </row>
@@ -2428,7 +2454,7 @@
         <v>91</v>
       </c>
       <c r="D48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E48" s="3"/>
     </row>
@@ -2443,7 +2469,7 @@
         <v>92</v>
       </c>
       <c r="D49" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E49" s="3"/>
     </row>
@@ -2458,7 +2484,7 @@
         <v>95</v>
       </c>
       <c r="D50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E50" s="3"/>
     </row>
@@ -2473,7 +2499,7 @@
         <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E51" s="3"/>
     </row>
@@ -2488,7 +2514,7 @@
         <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E52" s="3"/>
     </row>
@@ -2503,7 +2529,7 @@
         <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E53" s="3"/>
     </row>
@@ -2518,7 +2544,7 @@
         <v>104</v>
       </c>
       <c r="D54" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E54" s="3"/>
     </row>
@@ -2533,7 +2559,7 @@
         <v>106</v>
       </c>
       <c r="D55" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E55" s="3"/>
     </row>
@@ -2548,7 +2574,7 @@
         <v>245</v>
       </c>
       <c r="D56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E56" s="3"/>
     </row>
@@ -2563,7 +2589,7 @@
         <v>110</v>
       </c>
       <c r="D57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E57" s="3"/>
     </row>
@@ -2578,7 +2604,7 @@
         <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E58" s="3"/>
     </row>
@@ -2593,7 +2619,7 @@
         <v>116</v>
       </c>
       <c r="D59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E59" s="3"/>
     </row>
@@ -2608,7 +2634,7 @@
         <v>119</v>
       </c>
       <c r="D60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E60" s="3"/>
     </row>
@@ -2623,7 +2649,7 @@
         <v>122</v>
       </c>
       <c r="D61" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E61" s="3"/>
     </row>
@@ -2638,7 +2664,7 @@
         <v>125</v>
       </c>
       <c r="D62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E62" s="3"/>
     </row>
@@ -2653,7 +2679,7 @@
         <v>128</v>
       </c>
       <c r="D63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E63" s="3"/>
     </row>
@@ -2668,7 +2694,7 @@
         <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E64" s="3"/>
     </row>
@@ -2683,7 +2709,7 @@
         <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E65" s="3"/>
     </row>
@@ -2698,7 +2724,7 @@
         <v>137</v>
       </c>
       <c r="D66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E66" s="3"/>
     </row>
@@ -2713,7 +2739,7 @@
         <v>140</v>
       </c>
       <c r="D67" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E67" s="3"/>
     </row>
@@ -2728,7 +2754,7 @@
         <v>142</v>
       </c>
       <c r="D68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E68" s="3"/>
     </row>
@@ -2743,7 +2769,7 @@
         <v>145</v>
       </c>
       <c r="D69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E69" s="3"/>
     </row>
@@ -2758,7 +2784,7 @@
         <v>244</v>
       </c>
       <c r="D70" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E70" s="3"/>
     </row>
@@ -2773,7 +2799,7 @@
         <v>150</v>
       </c>
       <c r="D71" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E71" s="3"/>
     </row>
@@ -2788,7 +2814,7 @@
         <v>153</v>
       </c>
       <c r="D72" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E72" s="3"/>
     </row>
@@ -2803,7 +2829,7 @@
         <v>156</v>
       </c>
       <c r="D73" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E73" s="3"/>
     </row>
@@ -2818,9 +2844,11 @@
         <v>159</v>
       </c>
       <c r="D74" t="s">
-        <v>265</v>
-      </c>
-      <c r="E74" s="3"/>
+        <v>264</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -2833,7 +2861,7 @@
         <v>246</v>
       </c>
       <c r="D75" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E75" s="3"/>
     </row>
@@ -2848,7 +2876,7 @@
         <v>164</v>
       </c>
       <c r="D76" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E76" s="3"/>
     </row>
@@ -2878,7 +2906,7 @@
         <v>170</v>
       </c>
       <c r="D78" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E78" s="3"/>
     </row>
@@ -2893,7 +2921,7 @@
         <v>173</v>
       </c>
       <c r="D79" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E79" s="3"/>
     </row>
@@ -2908,7 +2936,7 @@
         <v>248</v>
       </c>
       <c r="D80" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E80" s="3"/>
     </row>
@@ -2923,7 +2951,7 @@
         <v>176</v>
       </c>
       <c r="D81" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E81" s="3"/>
     </row>
@@ -2938,7 +2966,7 @@
         <v>247</v>
       </c>
       <c r="D82" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E82" s="3"/>
     </row>
@@ -2953,7 +2981,7 @@
         <v>181</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E83" s="3"/>
     </row>
@@ -2968,7 +2996,7 @@
         <v>184</v>
       </c>
       <c r="D84" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E84" s="3"/>
     </row>
@@ -2983,7 +3011,7 @@
         <v>186</v>
       </c>
       <c r="D85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E85" s="3"/>
     </row>
@@ -2998,7 +3026,7 @@
         <v>189</v>
       </c>
       <c r="D86" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E86" s="3"/>
     </row>
@@ -3013,7 +3041,7 @@
         <v>192</v>
       </c>
       <c r="D87" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E87" s="3"/>
     </row>
@@ -3043,7 +3071,7 @@
         <v>197</v>
       </c>
       <c r="D89" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E89" s="3"/>
     </row>
@@ -3058,7 +3086,7 @@
         <v>199</v>
       </c>
       <c r="D90" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E90" s="3"/>
     </row>
@@ -3073,7 +3101,7 @@
         <v>202</v>
       </c>
       <c r="D91" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E91" s="3"/>
     </row>
@@ -3088,7 +3116,7 @@
         <v>205</v>
       </c>
       <c r="D92" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E92" s="3"/>
     </row>
@@ -3103,7 +3131,7 @@
         <v>207</v>
       </c>
       <c r="D93" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E93" s="3"/>
     </row>
@@ -3118,7 +3146,7 @@
         <v>209</v>
       </c>
       <c r="D94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E94" s="3"/>
     </row>
@@ -3133,7 +3161,7 @@
         <v>211</v>
       </c>
       <c r="D95" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E95" s="3"/>
     </row>
@@ -3148,7 +3176,7 @@
         <v>214</v>
       </c>
       <c r="D96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E96" s="3"/>
     </row>
@@ -3163,7 +3191,7 @@
         <v>216</v>
       </c>
       <c r="D97" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E97" s="3"/>
     </row>
@@ -3178,7 +3206,7 @@
         <v>219</v>
       </c>
       <c r="D98" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E98" s="3"/>
     </row>
@@ -3193,7 +3221,7 @@
         <v>222</v>
       </c>
       <c r="D99" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E99" s="3"/>
     </row>
@@ -3208,7 +3236,7 @@
         <v>224</v>
       </c>
       <c r="D100" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E100" s="3"/>
     </row>
@@ -3223,7 +3251,7 @@
         <v>226</v>
       </c>
       <c r="D101" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E101" s="3"/>
     </row>
@@ -3232,7 +3260,7 @@
         <v>252</v>
       </c>
       <c r="D102" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -3245,18 +3273,58 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C104" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D104" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C105" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D105" t="s">
-        <v>258</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C106" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D106" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C107" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D107" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C108" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D108" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C109" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D109" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C110" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D110" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3272,6 +3340,11 @@
     <hyperlink ref="C103" r:id="rId9" xr:uid="{21476635-8A57-BF48-A6EE-9245961D3107}"/>
     <hyperlink ref="C104" r:id="rId10" xr:uid="{587DFB68-236C-E049-803E-90B15C534CD5}"/>
     <hyperlink ref="C105" r:id="rId11" xr:uid="{4E49A6E5-716F-3843-B5F1-DCE3287ABAEC}"/>
+    <hyperlink ref="C106" r:id="rId12" xr:uid="{8E867387-8976-724E-A68E-220AE612DBDE}"/>
+    <hyperlink ref="C107" r:id="rId13" xr:uid="{BB0F2635-17C8-6E42-B38A-30D7ED4D235D}"/>
+    <hyperlink ref="C108" r:id="rId14" xr:uid="{9546D890-001E-5B41-8C3F-175C5B83627D}"/>
+    <hyperlink ref="C109" r:id="rId15" xr:uid="{3ECE3C3D-1691-8645-A60E-E1F112475EFD}"/>
+    <hyperlink ref="C110" r:id="rId16" xr:uid="{2BE2172B-A299-6246-99AC-20F1290CA8B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>